<commit_message>
menu system, correct fonts, RLE splash creator
</commit_message>
<xml_diff>
--- a/calc/Книга1.xlsx
+++ b/calc/Книга1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>PSC</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>bins with Fs/4</t>
+  </si>
+  <si>
+    <t>PWM bits</t>
+  </si>
+  <si>
+    <t>bit</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,6 +633,18 @@
         <v>25</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1">
+        <f>LOG(B3,2)</f>
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
menu system + splash RLE
</commit_message>
<xml_diff>
--- a/calc/Книга1.xlsx
+++ b/calc/Книга1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>PSC</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>bit</t>
+  </si>
+  <si>
+    <t>CW FFT width</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +455,7 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -465,51 +468,51 @@
       <c r="E1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>1024</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -524,7 +527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -539,7 +542,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -551,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -562,28 +565,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1">
         <f>B11/B4</f>
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f>B12*(1000/B7)</f>
-        <v>4.0960000000000001</v>
+        <v>8.1920000000000002</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -633,15 +636,27 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1">
+        <f>150/B18</f>
+        <v>1.2287999999999999</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B23" s="1">
         <f>LOG(B3,2)</f>
         <v>10</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>